<commit_message>
Update manual TCs for sort func
</commit_message>
<xml_diff>
--- a/UC02 SortSneakers_BossGiay_TCs.xlsx
+++ b/UC02 SortSneakers_BossGiay_TCs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SENIUM WITH JAVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16462A47-85B2-4CC5-94AC-1E014C44ECD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A794011-771C-425F-8E05-B594D67822EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{E28AEBC4-528C-4190-9FEA-BFE86C8B68D0}"/>
   </bookViews>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
   <si>
     <t>Environment</t>
   </si>
@@ -317,39 +317,37 @@
 - User has already triggered web browser</t>
   </si>
   <si>
-    <t>1. User navigates to the web URL via link: "https://bossgiay.vn/"</t>
-  </si>
-  <si>
-    <t>2. User clicks on the spy glass icon</t>
-  </si>
-  <si>
-    <t>4. User inputs clicks on spy glass icon or press enter key to conduct searching</t>
-  </si>
-  <si>
-    <t>5. User observes the returned listing of sneakers</t>
-  </si>
-  <si>
-    <t>Verify that user searches sneakers successfully when list of sneakers returned is less than two pages</t>
-  </si>
-  <si>
-    <t>- Test case is passed, the system returns a list of sneakers that is less than two pages
-- Taken screenshot:</t>
-  </si>
-  <si>
-    <t>Verify that user searches sneakers successfully when list of sneakers returned is more than one page</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>3. User inputs the $searchKey</t>
+    <t>Sort Sneakers</t>
+  </si>
+  <si>
+    <t>1. User navigates to the web URL via link: "https://bossgiay.vn/collections/all"</t>
+  </si>
+  <si>
+    <t>Verify that sort categories successfully with ascending price</t>
+  </si>
+  <si>
+    <t>sortCategories= {"Sneaker", "Slide/Sandal", "Bag", "Clothing"}</t>
+  </si>
+  <si>
+    <t>2. User clicks on $sortCategories on the left navigation of the website</t>
+  </si>
+  <si>
+    <t>3. User selects "Giá: Tăng dần" to sort product</t>
+  </si>
+  <si>
+    <t>Verify that sort categories successfully with descending price</t>
+  </si>
+  <si>
+    <t>3. User selects "Giá: Giảm dần" to sort product</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">- The system navigates user to web URL: "https://bossgiay.vn/"
-- The system displays the list of sneakers that is less than two pages:
-+ Each row of returned sneakers contains 4 sneakers
-+ Name of returned sneakers have to encompass the $searchKey without case sensitivity
+      <t xml:space="preserve">- The system navigates user to web URL: "https://bossgiay.vn/collections/all"
+- Pagination will be displayed when the returned list is more than one page
+- Product price is sorted by ascending value from lowest to highest
 </t>
     </r>
     <r>
@@ -360,7 +358,43 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>- Searching sneakers with one page successfully!</t>
+      <t>- Sort categories with ascending price successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify that sort categories by name successfully with ascending characters from A to Z</t>
+  </si>
+  <si>
+    <t>3. User selects "Tên: A-Z" to sort product</t>
+  </si>
+  <si>
+    <t>4. User observes the returned listing of product</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- The system navigates user to web URL: "https://bossgiay.vn/collections/all"
+- Pagination will be displayed when the returned list is more than one page
+- Product price is sorted by descending value from highest to lowest
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Sort categories with descending price successfully!</t>
     </r>
     <r>
       <rPr>
@@ -374,12 +408,9 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">- The system navigates user to web URL: "https://bossgiay.vn/"
-- The system displays the list of sneakers that is more than one page:
-+ Each row of returned sneakers contains 4 sneakers
-+ There is up to 50 sneakers per page
-+ Name of returned sneakers have to encompass the $searchKey without case sensitivity
-+ Pagination is shown contains ordinal numbers in the accordance with the returned total sneakers, previous and next button to facilate navigating among pages
+      <t xml:space="preserve">- The system navigates user to web URL: "https://bossgiay.vn/collections/all"
+- Pagination will be displayed when the returned list is more than one page
+- Product price is sorted by ascending characters from A to Z in the accordance with ASCII order
 </t>
     </r>
     <r>
@@ -390,7 +421,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>- Searching sneakers with more than one page successfully!</t>
+      <t>- Sort categories with ascending characters order successfully!</t>
     </r>
     <r>
       <rPr>
@@ -403,20 +434,16 @@
     </r>
   </si>
   <si>
-    <t>searchKey in the array {"A", "B", "S", "N", "M"}</t>
+    <t>Verify that sort categories by name successfully with ascending characters from Z to A</t>
   </si>
   <si>
-    <t>Verify that user searches sneakers unsuccessfully when search key does not match any sneakers</t>
-  </si>
-  <si>
-    <t>5. User observes the message: "Không tìm thấy nội dung bạn yêu cầu"</t>
+    <t>3. User selects "Tên: Z-A" to sort product</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">- The system navigates user to web URL: "https://bossgiay.vn/"
-- The system displays an alert message: 
-+ Không tìm thấy nội dung bạn yêu cầu
-+ Không tìm thấy "$searchKey". Vui lòng kiểm tra chính tả, sử dụng các từ tổng quát hơn và thử lại!
+      <t xml:space="preserve">- The system navigates user to web URL: "https://bossgiay.vn/collections/all"
+- Pagination will be displayed when the returned list is more than one page
+- Product price is sorted by descending characters from Z to A in the accordance with ASCII order
 </t>
     </r>
     <r>
@@ -427,7 +454,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>- Searching sneakers unsuccessfully because there is no sneakers match the inputted search key!</t>
+      <t>- Sort categories with descending characters order successfully!</t>
     </r>
     <r>
       <rPr>
@@ -438,23 +465,6 @@
       <t xml:space="preserve">
 </t>
     </r>
-  </si>
-  <si>
-    <t>searchKey in the array {"JORDAN", "LOW", "MID", "STAN", "NIKE", "ADIDAS", "SUPER", "HOLOGRAM", "DOMBA", "WHITE",       "BLACK", "RAINBOWN", "SMITH", "ALL", "MAX", "VICTOR", "MLB", "SHADOW", "DOGGER", "SLIDE", "GOLD", "HIGH", "ICE", "META", "LASER", "RED", "SIMPSONS", "ADLV", "BIG", "X", "V", "PUMA", "JAN", "K", "YANKEE", "MONOGRAM", "FORCE", "FRUIT", "ROSE", "CARTOON", "POUCH", "WORLDWIDE", "ASUNA", "JACQUARD", "F", "MON", "HOODY", "LIFE", "VOLT", "METALLIC", "POINT", "SP", "2", "SUNFLOWER", "SUPREME"};</t>
-  </si>
-  <si>
-    <t>searchKey in the array {"AJAX", "SOUL", "JORDAN NIGHT 1 LOW", "JORDAN NIGHT 1 SPADE", "KEY", "SAN", "SHALLOW", "WATT", "FORD", "BAM", "BANG", "JORLAN", "JORSAN", "JORFAN", "MC"}</t>
-  </si>
-  <si>
-    <t>- Test case is passed, the system returned all the expected messages
-- Taken screenshot:</t>
-  </si>
-  <si>
-    <t>- Test case is passed, the system returns a list of sneakers that is more than one page
-- Taken screenshot:</t>
-  </si>
-  <si>
-    <t>Sort Sneakers</t>
   </si>
 </sst>
 </file>
@@ -919,41 +929,8 @@
     <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="9" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -966,6 +943,39 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1662,10 +1672,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:AU197"/>
+  <dimension ref="A1:AU180"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H122" sqref="H122"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" outlineLevelRow="1"/>
@@ -1693,28 +1703,28 @@
     </row>
     <row r="2" spans="1:13" s="8" customFormat="1" ht="24.6">
       <c r="A2" s="11"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
       <c r="H2" s="12"/>
       <c r="M2" s="13"/>
     </row>
     <row r="3" spans="1:13" s="8" customFormat="1" ht="22.8">
       <c r="A3" s="11"/>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="47"/>
+      <c r="C3" s="59"/>
       <c r="D3" s="14"/>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="48"/>
+      <c r="G3" s="60"/>
       <c r="I3" s="14"/>
       <c r="J3" s="15"/>
       <c r="M3" s="13"/>
@@ -1723,11 +1733,11 @@
       <c r="A5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
+      <c r="B5" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -1741,11 +1751,11 @@
       <c r="A6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -1759,11 +1769,11 @@
       <c r="A7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
@@ -1777,11 +1787,11 @@
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
@@ -1795,11 +1805,11 @@
       <c r="A9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
@@ -1813,11 +1823,11 @@
       <c r="A10" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="53">
+      <c r="B10" s="56">
         <v>44532</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
@@ -1831,9 +1841,9 @@
       <c r="A11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
@@ -1875,27 +1885,27 @@
         <v>Build1</v>
       </c>
       <c r="B14" s="25">
-        <f t="shared" ref="B14:G14" si="0">COUNTIF($L$23:$L$48524,B13)</f>
+        <f>COUNTIF($L$23:$L$48507,B13)</f>
         <v>0</v>
       </c>
       <c r="C14" s="25">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($L$23:$L$48507,C13)</f>
         <v>0</v>
       </c>
       <c r="D14" s="25">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($L$23:$L$48507,D13)</f>
         <v>0</v>
       </c>
       <c r="E14" s="25">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($L$23:$L$48507,E13)</f>
         <v>0</v>
       </c>
       <c r="F14" s="25">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($L$23:$L$48507,F13)</f>
         <v>0</v>
       </c>
       <c r="G14" s="25">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($L$23:$L$48507,G13)</f>
         <v>0</v>
       </c>
       <c r="H14" s="26"/>
@@ -1910,27 +1920,27 @@
         <v>Build2</v>
       </c>
       <c r="B15" s="25">
-        <f t="shared" ref="B15:G15" si="1">COUNTIF($K$23:$K$48524,B13)</f>
+        <f>COUNTIF($K$23:$K$48507,B13)</f>
         <v>0</v>
       </c>
       <c r="C15" s="25">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($K$23:$K$48507,C13)</f>
         <v>0</v>
       </c>
       <c r="D15" s="25">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($K$23:$K$48507,D13)</f>
         <v>0</v>
       </c>
       <c r="E15" s="25">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($K$23:$K$48507,E13)</f>
         <v>0</v>
       </c>
       <c r="F15" s="25">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($K$23:$K$48507,F13)</f>
         <v>0</v>
       </c>
       <c r="G15" s="25">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($K$23:$K$48507,G13)</f>
         <v>0</v>
       </c>
       <c r="H15" s="26"/>
@@ -1945,27 +1955,27 @@
         <v>Build3</v>
       </c>
       <c r="B16" s="25">
-        <f>COUNTIF($J$23:$J$48524,B13)</f>
+        <f>COUNTIF($J$23:$J$48507,B13)</f>
         <v>0</v>
       </c>
       <c r="C16" s="25">
-        <f>COUNTIF($J$23:$J$48524,C13)</f>
+        <f>COUNTIF($J$23:$J$48507,C13)</f>
         <v>0</v>
       </c>
       <c r="D16" s="25">
-        <f>COUNTIF($J$23:$J$48524,D13)</f>
+        <f>COUNTIF($J$23:$J$48507,D13)</f>
         <v>0</v>
       </c>
       <c r="E16" s="25">
-        <f>COUNTIF($J$23:$J$48524,E13)</f>
+        <f>COUNTIF($J$23:$J$48507,E13)</f>
         <v>0</v>
       </c>
       <c r="F16" s="25">
-        <f>COUNTIF($J$23:$J$48524,F13)</f>
+        <f>COUNTIF($J$23:$J$48507,F13)</f>
         <v>0</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H16" s="26"/>
       <c r="I16" s="26"/>
@@ -1979,27 +1989,27 @@
         <v>Build4</v>
       </c>
       <c r="B17" s="25">
-        <f>COUNTIF($I$23:$I$48524,B13)</f>
+        <f>COUNTIF($I$23:$I$48507,B13)</f>
         <v>0</v>
       </c>
       <c r="C17" s="25">
-        <f>COUNTIF($I$23:$I$48524,C16)</f>
+        <f>COUNTIF($I$23:$I$48507,C16)</f>
         <v>0</v>
       </c>
       <c r="D17" s="25">
-        <f>COUNTIF($I$23:$I$48524,D13)</f>
+        <f>COUNTIF($I$23:$I$48507,D13)</f>
         <v>0</v>
       </c>
       <c r="E17" s="25">
-        <f>COUNTIF($I$23:$I$48524,E13)</f>
+        <f>COUNTIF($I$23:$I$48507,E13)</f>
         <v>0</v>
       </c>
       <c r="F17" s="25">
-        <f>COUNTIF($I$23:$I$48524,F13)</f>
+        <f>COUNTIF($I$23:$I$48507,F13)</f>
         <v>0</v>
       </c>
       <c r="G17" s="25">
-        <f>COUNTIF($I$23:$I$48524,G13)</f>
+        <f>COUNTIF($I$23:$I$48507,G13)</f>
         <v>0</v>
       </c>
       <c r="H17" s="26"/>
@@ -2014,27 +2024,27 @@
         <v>Build5</v>
       </c>
       <c r="B18" s="25">
-        <f t="shared" ref="B18:G18" si="2">COUNTIF($H$23:$H$48524,B13)</f>
-        <v>3</v>
+        <f>COUNTIF($H$23:$H$48507,B13)</f>
+        <v>4</v>
       </c>
       <c r="C18" s="25">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($H$23:$H$48507,C13)</f>
         <v>0</v>
       </c>
       <c r="D18" s="25">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($H$23:$H$48507,D13)</f>
         <v>0</v>
       </c>
       <c r="E18" s="25">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($H$23:$H$48507,E13)</f>
         <v>0</v>
       </c>
       <c r="F18" s="25">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($H$23:$H$48507,F13)</f>
         <v>0</v>
       </c>
       <c r="G18" s="25">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($H$23:$H$48507,G13)</f>
         <v>0</v>
       </c>
       <c r="H18" s="26"/>
@@ -2048,27 +2058,27 @@
         <v>24</v>
       </c>
       <c r="B19" s="28">
-        <f t="shared" ref="B19:G19" si="3">SUM(B14:B18)</f>
-        <v>3</v>
+        <f t="shared" ref="B19:G19" si="0">SUM(B14:B18)</f>
+        <v>4</v>
       </c>
       <c r="C19" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D19" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E19" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F19" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G19" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H19" s="26"/>
@@ -2096,13 +2106,13 @@
       <c r="E21" s="31"/>
       <c r="F21" s="31"/>
       <c r="G21" s="31"/>
-      <c r="H21" s="54" t="s">
+      <c r="H21" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
     </row>
     <row r="22" spans="1:12" s="30" customFormat="1" ht="13.2">
       <c r="A22" s="32" t="s">
@@ -2146,11 +2156,11 @@
       <c r="A23" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="52"/>
+      <c r="B23" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="53"/>
+      <c r="D23" s="54"/>
       <c r="E23" s="34"/>
       <c r="F23" s="34"/>
       <c r="G23" s="34"/>
@@ -2163,406 +2173,344 @@
       <c r="L23" s="36"/>
     </row>
     <row r="24" spans="1:12" s="37" customFormat="1" ht="52.2" customHeight="1" outlineLevel="1">
-      <c r="A24" s="57"/>
-      <c r="B24" s="58" t="s">
+      <c r="A24" s="46"/>
+      <c r="B24" s="47" t="s">
         <v>48</v>
       </c>
       <c r="C24" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="60" t="s">
+      <c r="E24" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="45"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="45"/>
+    </row>
+    <row r="25" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
+      <c r="A25" s="46"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="48"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="45"/>
+    </row>
+    <row r="26" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
+      <c r="A26" s="46"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="48"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="45"/>
+    </row>
+    <row r="27" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
+      <c r="A27" s="46"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="48"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="45"/>
+    </row>
+    <row r="28" spans="1:12" s="18" customFormat="1" ht="13.2">
+      <c r="A28" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="53"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="36"/>
+    </row>
+    <row r="29" spans="1:12" s="37" customFormat="1" ht="52.2" customHeight="1" outlineLevel="1">
+      <c r="A29" s="46"/>
+      <c r="B29" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="45"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+    </row>
+    <row r="30" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
+      <c r="A30" s="46"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="48"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="45"/>
+    </row>
+    <row r="31" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
+      <c r="A31" s="46"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="48"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="45"/>
+    </row>
+    <row r="32" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
+      <c r="A32" s="46"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="48"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="45"/>
+    </row>
+    <row r="33" spans="1:47" s="18" customFormat="1" ht="13.2">
+      <c r="A33" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="53"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="I33" s="36"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+    </row>
+    <row r="34" spans="1:47" s="37" customFormat="1" ht="52.2" customHeight="1" outlineLevel="1">
+      <c r="A34" s="46"/>
+      <c r="B34" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="45"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="45"/>
+      <c r="L34" s="45"/>
+    </row>
+    <row r="35" spans="1:47" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
+      <c r="A35" s="46"/>
+      <c r="B35" s="47"/>
+      <c r="C35" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="48"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="45"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="45"/>
+    </row>
+    <row r="36" spans="1:47" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
+      <c r="A36" s="46"/>
+      <c r="B36" s="47"/>
+      <c r="C36" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="48"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="51"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="45"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="45"/>
+    </row>
+    <row r="37" spans="1:47" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
+      <c r="A37" s="46"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" s="48"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="45"/>
+    </row>
+    <row r="38" spans="1:47" s="18" customFormat="1" ht="13.2">
+      <c r="A38" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="F24" s="49"/>
-      <c r="G24" s="55" t="s">
+      <c r="C38" s="53"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="34"/>
+      <c r="H38" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="36"/>
+      <c r="L38" s="36"/>
+    </row>
+    <row r="39" spans="1:47" s="37" customFormat="1" ht="52.2" customHeight="1" outlineLevel="1">
+      <c r="A39" s="46"/>
+      <c r="B39" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="F39" s="45"/>
+      <c r="G39" s="50"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="45"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="45"/>
+      <c r="L39" s="45"/>
+    </row>
+    <row r="40" spans="1:47" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
+      <c r="A40" s="46"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="H24" s="56"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-    </row>
-    <row r="25" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A25" s="57"/>
-      <c r="B25" s="58"/>
-      <c r="C25" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" s="59"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
-    </row>
-    <row r="26" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A26" s="57"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="59"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="49"/>
-    </row>
-    <row r="27" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A27" s="57"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="59"/>
-      <c r="E27" s="60"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="49"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="49"/>
-    </row>
-    <row r="28" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A28" s="57"/>
-      <c r="B28" s="58"/>
-      <c r="C28" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="59"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="49"/>
-      <c r="L28" s="49"/>
-    </row>
-    <row r="29" spans="1:12" s="18" customFormat="1" ht="13.2">
-      <c r="A29" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="50" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="51"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="36"/>
-    </row>
-    <row r="30" spans="1:12" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A30" s="57"/>
-      <c r="B30" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="E30" s="60" t="s">
-        <v>60</v>
-      </c>
-      <c r="F30" s="49"/>
-      <c r="G30" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="H30" s="56"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="49"/>
-    </row>
-    <row r="31" spans="1:12" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A31" s="57"/>
-      <c r="B31" s="58"/>
-      <c r="C31" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="59"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="49"/>
-      <c r="K31" s="49"/>
-      <c r="L31" s="49"/>
-    </row>
-    <row r="32" spans="1:12" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A32" s="57"/>
-      <c r="B32" s="58"/>
-      <c r="C32" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="D32" s="59"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="49"/>
-      <c r="K32" s="49"/>
-      <c r="L32" s="49"/>
-    </row>
-    <row r="33" spans="1:47" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A33" s="57"/>
-      <c r="B33" s="58"/>
-      <c r="C33" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" s="59"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="49"/>
-      <c r="K33" s="49"/>
-      <c r="L33" s="49"/>
-    </row>
-    <row r="34" spans="1:47" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A34" s="57"/>
-      <c r="B34" s="58"/>
-      <c r="C34" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" s="59"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="55"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="49"/>
-      <c r="J34" s="49"/>
-      <c r="K34" s="49"/>
-      <c r="L34" s="49"/>
-    </row>
-    <row r="35" spans="1:47" s="18" customFormat="1" ht="13.2">
-      <c r="A35" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" s="50" t="s">
+      <c r="D40" s="48"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="50"/>
+      <c r="H40" s="51"/>
+      <c r="I40" s="45"/>
+      <c r="J40" s="45"/>
+      <c r="K40" s="45"/>
+      <c r="L40" s="45"/>
+    </row>
+    <row r="41" spans="1:47" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
+      <c r="A41" s="46"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" s="48"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="51"/>
+      <c r="I41" s="45"/>
+      <c r="J41" s="45"/>
+      <c r="K41" s="45"/>
+      <c r="L41" s="45"/>
+    </row>
+    <row r="42" spans="1:47" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
+      <c r="A42" s="46"/>
+      <c r="B42" s="47"/>
+      <c r="C42" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="51"/>
-      <c r="D35" s="52"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="I35" s="36"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="36"/>
-    </row>
-    <row r="36" spans="1:47" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A36" s="57"/>
-      <c r="B36" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="59" t="s">
-        <v>63</v>
-      </c>
-      <c r="E36" s="60" t="s">
-        <v>65</v>
-      </c>
-      <c r="F36" s="49"/>
-      <c r="G36" s="55" t="s">
-        <v>66</v>
-      </c>
-      <c r="H36" s="56"/>
-      <c r="I36" s="49"/>
-      <c r="J36" s="49"/>
-      <c r="K36" s="49"/>
-      <c r="L36" s="49"/>
-    </row>
-    <row r="37" spans="1:47" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A37" s="57"/>
-      <c r="B37" s="58"/>
-      <c r="C37" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="59"/>
-      <c r="E37" s="60"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="49"/>
-      <c r="J37" s="49"/>
-      <c r="K37" s="49"/>
-      <c r="L37" s="49"/>
-    </row>
-    <row r="38" spans="1:47" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A38" s="57"/>
-      <c r="B38" s="58"/>
-      <c r="C38" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="D38" s="59"/>
-      <c r="E38" s="60"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="49"/>
-      <c r="J38" s="49"/>
-      <c r="K38" s="49"/>
-      <c r="L38" s="49"/>
-    </row>
-    <row r="39" spans="1:47" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A39" s="57"/>
-      <c r="B39" s="58"/>
-      <c r="C39" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="D39" s="59"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="49"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="49"/>
-      <c r="L39" s="49"/>
-    </row>
-    <row r="40" spans="1:47" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A40" s="57"/>
-      <c r="B40" s="58"/>
-      <c r="C40" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="D40" s="59"/>
-      <c r="E40" s="60"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="55"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="49"/>
-      <c r="J40" s="49"/>
-      <c r="K40" s="49"/>
-      <c r="L40" s="49"/>
-    </row>
-    <row r="41" spans="1:47">
-      <c r="A41" s="39"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="39"/>
-      <c r="J41" s="39"/>
-      <c r="K41" s="39"/>
-      <c r="L41" s="39"/>
-      <c r="M41" s="39"/>
-      <c r="N41" s="39"/>
-      <c r="O41" s="39"/>
-      <c r="P41" s="39"/>
-      <c r="Q41" s="39"/>
-      <c r="R41" s="39"/>
-      <c r="S41" s="39"/>
-      <c r="T41" s="39"/>
-      <c r="U41" s="39"/>
-      <c r="V41" s="39"/>
-      <c r="W41" s="39"/>
-      <c r="X41" s="39"/>
-      <c r="Y41" s="39"/>
-      <c r="Z41" s="39"/>
-      <c r="AA41" s="39"/>
-      <c r="AB41" s="39"/>
-      <c r="AC41" s="39"/>
-      <c r="AD41" s="39"/>
-      <c r="AE41" s="39"/>
-      <c r="AF41" s="39"/>
-      <c r="AG41" s="39"/>
-      <c r="AH41" s="39"/>
-      <c r="AI41" s="39"/>
-      <c r="AJ41" s="39"/>
-      <c r="AK41" s="39"/>
-      <c r="AL41" s="39"/>
-      <c r="AM41" s="39"/>
-      <c r="AN41" s="39"/>
-      <c r="AO41" s="39"/>
-      <c r="AP41" s="39"/>
-      <c r="AQ41" s="39"/>
-      <c r="AR41" s="39"/>
-      <c r="AS41" s="39"/>
-      <c r="AT41" s="39"/>
-      <c r="AU41" s="39"/>
-    </row>
-    <row r="42" spans="1:47">
-      <c r="A42" s="39"/>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
-      <c r="K42" s="39"/>
-      <c r="L42" s="39"/>
-      <c r="M42" s="39"/>
-      <c r="N42" s="39"/>
-      <c r="O42" s="39"/>
-      <c r="P42" s="39"/>
-      <c r="Q42" s="39"/>
-      <c r="R42" s="39"/>
-      <c r="S42" s="39"/>
-      <c r="T42" s="39"/>
-      <c r="U42" s="39"/>
-      <c r="V42" s="39"/>
-      <c r="W42" s="39"/>
-      <c r="X42" s="39"/>
-      <c r="Y42" s="39"/>
-      <c r="Z42" s="39"/>
-      <c r="AA42" s="39"/>
-      <c r="AB42" s="39"/>
-      <c r="AC42" s="39"/>
-      <c r="AD42" s="39"/>
-      <c r="AE42" s="39"/>
-      <c r="AF42" s="39"/>
-      <c r="AG42" s="39"/>
-      <c r="AH42" s="39"/>
-      <c r="AI42" s="39"/>
-      <c r="AJ42" s="39"/>
-      <c r="AK42" s="39"/>
-      <c r="AL42" s="39"/>
-      <c r="AM42" s="39"/>
-      <c r="AN42" s="39"/>
-      <c r="AO42" s="39"/>
-      <c r="AP42" s="39"/>
-      <c r="AQ42" s="39"/>
-      <c r="AR42" s="39"/>
-      <c r="AS42" s="39"/>
-      <c r="AT42" s="39"/>
-      <c r="AU42" s="39"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="51"/>
+      <c r="I42" s="45"/>
+      <c r="J42" s="45"/>
+      <c r="K42" s="45"/>
+      <c r="L42" s="45"/>
     </row>
     <row r="43" spans="1:47">
       <c r="A43" s="39"/>
@@ -9326,906 +9274,85 @@
       <c r="AT180" s="39"/>
       <c r="AU180" s="39"/>
     </row>
-    <row r="181" spans="1:47">
-      <c r="A181" s="39"/>
-      <c r="B181" s="39"/>
-      <c r="C181" s="39"/>
-      <c r="D181" s="39"/>
-      <c r="E181" s="39"/>
-      <c r="F181" s="39"/>
-      <c r="G181" s="39"/>
-      <c r="H181" s="39"/>
-      <c r="I181" s="39"/>
-      <c r="J181" s="39"/>
-      <c r="K181" s="39"/>
-      <c r="L181" s="39"/>
-      <c r="M181" s="39"/>
-      <c r="N181" s="39"/>
-      <c r="O181" s="39"/>
-      <c r="P181" s="39"/>
-      <c r="Q181" s="39"/>
-      <c r="R181" s="39"/>
-      <c r="S181" s="39"/>
-      <c r="T181" s="39"/>
-      <c r="U181" s="39"/>
-      <c r="V181" s="39"/>
-      <c r="W181" s="39"/>
-      <c r="X181" s="39"/>
-      <c r="Y181" s="39"/>
-      <c r="Z181" s="39"/>
-      <c r="AA181" s="39"/>
-      <c r="AB181" s="39"/>
-      <c r="AC181" s="39"/>
-      <c r="AD181" s="39"/>
-      <c r="AE181" s="39"/>
-      <c r="AF181" s="39"/>
-      <c r="AG181" s="39"/>
-      <c r="AH181" s="39"/>
-      <c r="AI181" s="39"/>
-      <c r="AJ181" s="39"/>
-      <c r="AK181" s="39"/>
-      <c r="AL181" s="39"/>
-      <c r="AM181" s="39"/>
-      <c r="AN181" s="39"/>
-      <c r="AO181" s="39"/>
-      <c r="AP181" s="39"/>
-      <c r="AQ181" s="39"/>
-      <c r="AR181" s="39"/>
-      <c r="AS181" s="39"/>
-      <c r="AT181" s="39"/>
-      <c r="AU181" s="39"/>
-    </row>
-    <row r="182" spans="1:47">
-      <c r="A182" s="39"/>
-      <c r="B182" s="39"/>
-      <c r="C182" s="39"/>
-      <c r="D182" s="39"/>
-      <c r="E182" s="39"/>
-      <c r="F182" s="39"/>
-      <c r="G182" s="39"/>
-      <c r="H182" s="39"/>
-      <c r="I182" s="39"/>
-      <c r="J182" s="39"/>
-      <c r="K182" s="39"/>
-      <c r="L182" s="39"/>
-      <c r="M182" s="39"/>
-      <c r="N182" s="39"/>
-      <c r="O182" s="39"/>
-      <c r="P182" s="39"/>
-      <c r="Q182" s="39"/>
-      <c r="R182" s="39"/>
-      <c r="S182" s="39"/>
-      <c r="T182" s="39"/>
-      <c r="U182" s="39"/>
-      <c r="V182" s="39"/>
-      <c r="W182" s="39"/>
-      <c r="X182" s="39"/>
-      <c r="Y182" s="39"/>
-      <c r="Z182" s="39"/>
-      <c r="AA182" s="39"/>
-      <c r="AB182" s="39"/>
-      <c r="AC182" s="39"/>
-      <c r="AD182" s="39"/>
-      <c r="AE182" s="39"/>
-      <c r="AF182" s="39"/>
-      <c r="AG182" s="39"/>
-      <c r="AH182" s="39"/>
-      <c r="AI182" s="39"/>
-      <c r="AJ182" s="39"/>
-      <c r="AK182" s="39"/>
-      <c r="AL182" s="39"/>
-      <c r="AM182" s="39"/>
-      <c r="AN182" s="39"/>
-      <c r="AO182" s="39"/>
-      <c r="AP182" s="39"/>
-      <c r="AQ182" s="39"/>
-      <c r="AR182" s="39"/>
-      <c r="AS182" s="39"/>
-      <c r="AT182" s="39"/>
-      <c r="AU182" s="39"/>
-    </row>
-    <row r="183" spans="1:47">
-      <c r="A183" s="39"/>
-      <c r="B183" s="39"/>
-      <c r="C183" s="39"/>
-      <c r="D183" s="39"/>
-      <c r="E183" s="39"/>
-      <c r="F183" s="39"/>
-      <c r="G183" s="39"/>
-      <c r="H183" s="39"/>
-      <c r="I183" s="39"/>
-      <c r="J183" s="39"/>
-      <c r="K183" s="39"/>
-      <c r="L183" s="39"/>
-      <c r="M183" s="39"/>
-      <c r="N183" s="39"/>
-      <c r="O183" s="39"/>
-      <c r="P183" s="39"/>
-      <c r="Q183" s="39"/>
-      <c r="R183" s="39"/>
-      <c r="S183" s="39"/>
-      <c r="T183" s="39"/>
-      <c r="U183" s="39"/>
-      <c r="V183" s="39"/>
-      <c r="W183" s="39"/>
-      <c r="X183" s="39"/>
-      <c r="Y183" s="39"/>
-      <c r="Z183" s="39"/>
-      <c r="AA183" s="39"/>
-      <c r="AB183" s="39"/>
-      <c r="AC183" s="39"/>
-      <c r="AD183" s="39"/>
-      <c r="AE183" s="39"/>
-      <c r="AF183" s="39"/>
-      <c r="AG183" s="39"/>
-      <c r="AH183" s="39"/>
-      <c r="AI183" s="39"/>
-      <c r="AJ183" s="39"/>
-      <c r="AK183" s="39"/>
-      <c r="AL183" s="39"/>
-      <c r="AM183" s="39"/>
-      <c r="AN183" s="39"/>
-      <c r="AO183" s="39"/>
-      <c r="AP183" s="39"/>
-      <c r="AQ183" s="39"/>
-      <c r="AR183" s="39"/>
-      <c r="AS183" s="39"/>
-      <c r="AT183" s="39"/>
-      <c r="AU183" s="39"/>
-    </row>
-    <row r="184" spans="1:47">
-      <c r="A184" s="39"/>
-      <c r="B184" s="39"/>
-      <c r="C184" s="39"/>
-      <c r="D184" s="39"/>
-      <c r="E184" s="39"/>
-      <c r="F184" s="39"/>
-      <c r="G184" s="39"/>
-      <c r="H184" s="39"/>
-      <c r="I184" s="39"/>
-      <c r="J184" s="39"/>
-      <c r="K184" s="39"/>
-      <c r="L184" s="39"/>
-      <c r="M184" s="39"/>
-      <c r="N184" s="39"/>
-      <c r="O184" s="39"/>
-      <c r="P184" s="39"/>
-      <c r="Q184" s="39"/>
-      <c r="R184" s="39"/>
-      <c r="S184" s="39"/>
-      <c r="T184" s="39"/>
-      <c r="U184" s="39"/>
-      <c r="V184" s="39"/>
-      <c r="W184" s="39"/>
-      <c r="X184" s="39"/>
-      <c r="Y184" s="39"/>
-      <c r="Z184" s="39"/>
-      <c r="AA184" s="39"/>
-      <c r="AB184" s="39"/>
-      <c r="AC184" s="39"/>
-      <c r="AD184" s="39"/>
-      <c r="AE184" s="39"/>
-      <c r="AF184" s="39"/>
-      <c r="AG184" s="39"/>
-      <c r="AH184" s="39"/>
-      <c r="AI184" s="39"/>
-      <c r="AJ184" s="39"/>
-      <c r="AK184" s="39"/>
-      <c r="AL184" s="39"/>
-      <c r="AM184" s="39"/>
-      <c r="AN184" s="39"/>
-      <c r="AO184" s="39"/>
-      <c r="AP184" s="39"/>
-      <c r="AQ184" s="39"/>
-      <c r="AR184" s="39"/>
-      <c r="AS184" s="39"/>
-      <c r="AT184" s="39"/>
-      <c r="AU184" s="39"/>
-    </row>
-    <row r="185" spans="1:47">
-      <c r="A185" s="39"/>
-      <c r="B185" s="39"/>
-      <c r="C185" s="39"/>
-      <c r="D185" s="39"/>
-      <c r="E185" s="39"/>
-      <c r="F185" s="39"/>
-      <c r="G185" s="39"/>
-      <c r="H185" s="39"/>
-      <c r="I185" s="39"/>
-      <c r="J185" s="39"/>
-      <c r="K185" s="39"/>
-      <c r="L185" s="39"/>
-      <c r="M185" s="39"/>
-      <c r="N185" s="39"/>
-      <c r="O185" s="39"/>
-      <c r="P185" s="39"/>
-      <c r="Q185" s="39"/>
-      <c r="R185" s="39"/>
-      <c r="S185" s="39"/>
-      <c r="T185" s="39"/>
-      <c r="U185" s="39"/>
-      <c r="V185" s="39"/>
-      <c r="W185" s="39"/>
-      <c r="X185" s="39"/>
-      <c r="Y185" s="39"/>
-      <c r="Z185" s="39"/>
-      <c r="AA185" s="39"/>
-      <c r="AB185" s="39"/>
-      <c r="AC185" s="39"/>
-      <c r="AD185" s="39"/>
-      <c r="AE185" s="39"/>
-      <c r="AF185" s="39"/>
-      <c r="AG185" s="39"/>
-      <c r="AH185" s="39"/>
-      <c r="AI185" s="39"/>
-      <c r="AJ185" s="39"/>
-      <c r="AK185" s="39"/>
-      <c r="AL185" s="39"/>
-      <c r="AM185" s="39"/>
-      <c r="AN185" s="39"/>
-      <c r="AO185" s="39"/>
-      <c r="AP185" s="39"/>
-      <c r="AQ185" s="39"/>
-      <c r="AR185" s="39"/>
-      <c r="AS185" s="39"/>
-      <c r="AT185" s="39"/>
-      <c r="AU185" s="39"/>
-    </row>
-    <row r="186" spans="1:47">
-      <c r="A186" s="39"/>
-      <c r="B186" s="39"/>
-      <c r="C186" s="39"/>
-      <c r="D186" s="39"/>
-      <c r="E186" s="39"/>
-      <c r="F186" s="39"/>
-      <c r="G186" s="39"/>
-      <c r="H186" s="39"/>
-      <c r="I186" s="39"/>
-      <c r="J186" s="39"/>
-      <c r="K186" s="39"/>
-      <c r="L186" s="39"/>
-      <c r="M186" s="39"/>
-      <c r="N186" s="39"/>
-      <c r="O186" s="39"/>
-      <c r="P186" s="39"/>
-      <c r="Q186" s="39"/>
-      <c r="R186" s="39"/>
-      <c r="S186" s="39"/>
-      <c r="T186" s="39"/>
-      <c r="U186" s="39"/>
-      <c r="V186" s="39"/>
-      <c r="W186" s="39"/>
-      <c r="X186" s="39"/>
-      <c r="Y186" s="39"/>
-      <c r="Z186" s="39"/>
-      <c r="AA186" s="39"/>
-      <c r="AB186" s="39"/>
-      <c r="AC186" s="39"/>
-      <c r="AD186" s="39"/>
-      <c r="AE186" s="39"/>
-      <c r="AF186" s="39"/>
-      <c r="AG186" s="39"/>
-      <c r="AH186" s="39"/>
-      <c r="AI186" s="39"/>
-      <c r="AJ186" s="39"/>
-      <c r="AK186" s="39"/>
-      <c r="AL186" s="39"/>
-      <c r="AM186" s="39"/>
-      <c r="AN186" s="39"/>
-      <c r="AO186" s="39"/>
-      <c r="AP186" s="39"/>
-      <c r="AQ186" s="39"/>
-      <c r="AR186" s="39"/>
-      <c r="AS186" s="39"/>
-      <c r="AT186" s="39"/>
-      <c r="AU186" s="39"/>
-    </row>
-    <row r="187" spans="1:47">
-      <c r="A187" s="39"/>
-      <c r="B187" s="39"/>
-      <c r="C187" s="39"/>
-      <c r="D187" s="39"/>
-      <c r="E187" s="39"/>
-      <c r="F187" s="39"/>
-      <c r="G187" s="39"/>
-      <c r="H187" s="39"/>
-      <c r="I187" s="39"/>
-      <c r="J187" s="39"/>
-      <c r="K187" s="39"/>
-      <c r="L187" s="39"/>
-      <c r="M187" s="39"/>
-      <c r="N187" s="39"/>
-      <c r="O187" s="39"/>
-      <c r="P187" s="39"/>
-      <c r="Q187" s="39"/>
-      <c r="R187" s="39"/>
-      <c r="S187" s="39"/>
-      <c r="T187" s="39"/>
-      <c r="U187" s="39"/>
-      <c r="V187" s="39"/>
-      <c r="W187" s="39"/>
-      <c r="X187" s="39"/>
-      <c r="Y187" s="39"/>
-      <c r="Z187" s="39"/>
-      <c r="AA187" s="39"/>
-      <c r="AB187" s="39"/>
-      <c r="AC187" s="39"/>
-      <c r="AD187" s="39"/>
-      <c r="AE187" s="39"/>
-      <c r="AF187" s="39"/>
-      <c r="AG187" s="39"/>
-      <c r="AH187" s="39"/>
-      <c r="AI187" s="39"/>
-      <c r="AJ187" s="39"/>
-      <c r="AK187" s="39"/>
-      <c r="AL187" s="39"/>
-      <c r="AM187" s="39"/>
-      <c r="AN187" s="39"/>
-      <c r="AO187" s="39"/>
-      <c r="AP187" s="39"/>
-      <c r="AQ187" s="39"/>
-      <c r="AR187" s="39"/>
-      <c r="AS187" s="39"/>
-      <c r="AT187" s="39"/>
-      <c r="AU187" s="39"/>
-    </row>
-    <row r="188" spans="1:47">
-      <c r="A188" s="39"/>
-      <c r="B188" s="39"/>
-      <c r="C188" s="39"/>
-      <c r="D188" s="39"/>
-      <c r="E188" s="39"/>
-      <c r="F188" s="39"/>
-      <c r="G188" s="39"/>
-      <c r="H188" s="39"/>
-      <c r="I188" s="39"/>
-      <c r="J188" s="39"/>
-      <c r="K188" s="39"/>
-      <c r="L188" s="39"/>
-      <c r="M188" s="39"/>
-      <c r="N188" s="39"/>
-      <c r="O188" s="39"/>
-      <c r="P188" s="39"/>
-      <c r="Q188" s="39"/>
-      <c r="R188" s="39"/>
-      <c r="S188" s="39"/>
-      <c r="T188" s="39"/>
-      <c r="U188" s="39"/>
-      <c r="V188" s="39"/>
-      <c r="W188" s="39"/>
-      <c r="X188" s="39"/>
-      <c r="Y188" s="39"/>
-      <c r="Z188" s="39"/>
-      <c r="AA188" s="39"/>
-      <c r="AB188" s="39"/>
-      <c r="AC188" s="39"/>
-      <c r="AD188" s="39"/>
-      <c r="AE188" s="39"/>
-      <c r="AF188" s="39"/>
-      <c r="AG188" s="39"/>
-      <c r="AH188" s="39"/>
-      <c r="AI188" s="39"/>
-      <c r="AJ188" s="39"/>
-      <c r="AK188" s="39"/>
-      <c r="AL188" s="39"/>
-      <c r="AM188" s="39"/>
-      <c r="AN188" s="39"/>
-      <c r="AO188" s="39"/>
-      <c r="AP188" s="39"/>
-      <c r="AQ188" s="39"/>
-      <c r="AR188" s="39"/>
-      <c r="AS188" s="39"/>
-      <c r="AT188" s="39"/>
-      <c r="AU188" s="39"/>
-    </row>
-    <row r="189" spans="1:47">
-      <c r="A189" s="39"/>
-      <c r="B189" s="39"/>
-      <c r="C189" s="39"/>
-      <c r="D189" s="39"/>
-      <c r="E189" s="39"/>
-      <c r="F189" s="39"/>
-      <c r="G189" s="39"/>
-      <c r="H189" s="39"/>
-      <c r="I189" s="39"/>
-      <c r="J189" s="39"/>
-      <c r="K189" s="39"/>
-      <c r="L189" s="39"/>
-      <c r="M189" s="39"/>
-      <c r="N189" s="39"/>
-      <c r="O189" s="39"/>
-      <c r="P189" s="39"/>
-      <c r="Q189" s="39"/>
-      <c r="R189" s="39"/>
-      <c r="S189" s="39"/>
-      <c r="T189" s="39"/>
-      <c r="U189" s="39"/>
-      <c r="V189" s="39"/>
-      <c r="W189" s="39"/>
-      <c r="X189" s="39"/>
-      <c r="Y189" s="39"/>
-      <c r="Z189" s="39"/>
-      <c r="AA189" s="39"/>
-      <c r="AB189" s="39"/>
-      <c r="AC189" s="39"/>
-      <c r="AD189" s="39"/>
-      <c r="AE189" s="39"/>
-      <c r="AF189" s="39"/>
-      <c r="AG189" s="39"/>
-      <c r="AH189" s="39"/>
-      <c r="AI189" s="39"/>
-      <c r="AJ189" s="39"/>
-      <c r="AK189" s="39"/>
-      <c r="AL189" s="39"/>
-      <c r="AM189" s="39"/>
-      <c r="AN189" s="39"/>
-      <c r="AO189" s="39"/>
-      <c r="AP189" s="39"/>
-      <c r="AQ189" s="39"/>
-      <c r="AR189" s="39"/>
-      <c r="AS189" s="39"/>
-      <c r="AT189" s="39"/>
-      <c r="AU189" s="39"/>
-    </row>
-    <row r="190" spans="1:47">
-      <c r="A190" s="39"/>
-      <c r="B190" s="39"/>
-      <c r="C190" s="39"/>
-      <c r="D190" s="39"/>
-      <c r="E190" s="39"/>
-      <c r="F190" s="39"/>
-      <c r="G190" s="39"/>
-      <c r="H190" s="39"/>
-      <c r="I190" s="39"/>
-      <c r="J190" s="39"/>
-      <c r="K190" s="39"/>
-      <c r="L190" s="39"/>
-      <c r="M190" s="39"/>
-      <c r="N190" s="39"/>
-      <c r="O190" s="39"/>
-      <c r="P190" s="39"/>
-      <c r="Q190" s="39"/>
-      <c r="R190" s="39"/>
-      <c r="S190" s="39"/>
-      <c r="T190" s="39"/>
-      <c r="U190" s="39"/>
-      <c r="V190" s="39"/>
-      <c r="W190" s="39"/>
-      <c r="X190" s="39"/>
-      <c r="Y190" s="39"/>
-      <c r="Z190" s="39"/>
-      <c r="AA190" s="39"/>
-      <c r="AB190" s="39"/>
-      <c r="AC190" s="39"/>
-      <c r="AD190" s="39"/>
-      <c r="AE190" s="39"/>
-      <c r="AF190" s="39"/>
-      <c r="AG190" s="39"/>
-      <c r="AH190" s="39"/>
-      <c r="AI190" s="39"/>
-      <c r="AJ190" s="39"/>
-      <c r="AK190" s="39"/>
-      <c r="AL190" s="39"/>
-      <c r="AM190" s="39"/>
-      <c r="AN190" s="39"/>
-      <c r="AO190" s="39"/>
-      <c r="AP190" s="39"/>
-      <c r="AQ190" s="39"/>
-      <c r="AR190" s="39"/>
-      <c r="AS190" s="39"/>
-      <c r="AT190" s="39"/>
-      <c r="AU190" s="39"/>
-    </row>
-    <row r="191" spans="1:47">
-      <c r="A191" s="39"/>
-      <c r="B191" s="39"/>
-      <c r="C191" s="39"/>
-      <c r="D191" s="39"/>
-      <c r="E191" s="39"/>
-      <c r="F191" s="39"/>
-      <c r="G191" s="39"/>
-      <c r="H191" s="39"/>
-      <c r="I191" s="39"/>
-      <c r="J191" s="39"/>
-      <c r="K191" s="39"/>
-      <c r="L191" s="39"/>
-      <c r="M191" s="39"/>
-      <c r="N191" s="39"/>
-      <c r="O191" s="39"/>
-      <c r="P191" s="39"/>
-      <c r="Q191" s="39"/>
-      <c r="R191" s="39"/>
-      <c r="S191" s="39"/>
-      <c r="T191" s="39"/>
-      <c r="U191" s="39"/>
-      <c r="V191" s="39"/>
-      <c r="W191" s="39"/>
-      <c r="X191" s="39"/>
-      <c r="Y191" s="39"/>
-      <c r="Z191" s="39"/>
-      <c r="AA191" s="39"/>
-      <c r="AB191" s="39"/>
-      <c r="AC191" s="39"/>
-      <c r="AD191" s="39"/>
-      <c r="AE191" s="39"/>
-      <c r="AF191" s="39"/>
-      <c r="AG191" s="39"/>
-      <c r="AH191" s="39"/>
-      <c r="AI191" s="39"/>
-      <c r="AJ191" s="39"/>
-      <c r="AK191" s="39"/>
-      <c r="AL191" s="39"/>
-      <c r="AM191" s="39"/>
-      <c r="AN191" s="39"/>
-      <c r="AO191" s="39"/>
-      <c r="AP191" s="39"/>
-      <c r="AQ191" s="39"/>
-      <c r="AR191" s="39"/>
-      <c r="AS191" s="39"/>
-      <c r="AT191" s="39"/>
-      <c r="AU191" s="39"/>
-    </row>
-    <row r="192" spans="1:47">
-      <c r="A192" s="39"/>
-      <c r="B192" s="39"/>
-      <c r="C192" s="39"/>
-      <c r="D192" s="39"/>
-      <c r="E192" s="39"/>
-      <c r="F192" s="39"/>
-      <c r="G192" s="39"/>
-      <c r="H192" s="39"/>
-      <c r="I192" s="39"/>
-      <c r="J192" s="39"/>
-      <c r="K192" s="39"/>
-      <c r="L192" s="39"/>
-      <c r="M192" s="39"/>
-      <c r="N192" s="39"/>
-      <c r="O192" s="39"/>
-      <c r="P192" s="39"/>
-      <c r="Q192" s="39"/>
-      <c r="R192" s="39"/>
-      <c r="S192" s="39"/>
-      <c r="T192" s="39"/>
-      <c r="U192" s="39"/>
-      <c r="V192" s="39"/>
-      <c r="W192" s="39"/>
-      <c r="X192" s="39"/>
-      <c r="Y192" s="39"/>
-      <c r="Z192" s="39"/>
-      <c r="AA192" s="39"/>
-      <c r="AB192" s="39"/>
-      <c r="AC192" s="39"/>
-      <c r="AD192" s="39"/>
-      <c r="AE192" s="39"/>
-      <c r="AF192" s="39"/>
-      <c r="AG192" s="39"/>
-      <c r="AH192" s="39"/>
-      <c r="AI192" s="39"/>
-      <c r="AJ192" s="39"/>
-      <c r="AK192" s="39"/>
-      <c r="AL192" s="39"/>
-      <c r="AM192" s="39"/>
-      <c r="AN192" s="39"/>
-      <c r="AO192" s="39"/>
-      <c r="AP192" s="39"/>
-      <c r="AQ192" s="39"/>
-      <c r="AR192" s="39"/>
-      <c r="AS192" s="39"/>
-      <c r="AT192" s="39"/>
-      <c r="AU192" s="39"/>
-    </row>
-    <row r="193" spans="1:47">
-      <c r="A193" s="39"/>
-      <c r="B193" s="39"/>
-      <c r="C193" s="39"/>
-      <c r="D193" s="39"/>
-      <c r="E193" s="39"/>
-      <c r="F193" s="39"/>
-      <c r="G193" s="39"/>
-      <c r="H193" s="39"/>
-      <c r="I193" s="39"/>
-      <c r="J193" s="39"/>
-      <c r="K193" s="39"/>
-      <c r="L193" s="39"/>
-      <c r="M193" s="39"/>
-      <c r="N193" s="39"/>
-      <c r="O193" s="39"/>
-      <c r="P193" s="39"/>
-      <c r="Q193" s="39"/>
-      <c r="R193" s="39"/>
-      <c r="S193" s="39"/>
-      <c r="T193" s="39"/>
-      <c r="U193" s="39"/>
-      <c r="V193" s="39"/>
-      <c r="W193" s="39"/>
-      <c r="X193" s="39"/>
-      <c r="Y193" s="39"/>
-      <c r="Z193" s="39"/>
-      <c r="AA193" s="39"/>
-      <c r="AB193" s="39"/>
-      <c r="AC193" s="39"/>
-      <c r="AD193" s="39"/>
-      <c r="AE193" s="39"/>
-      <c r="AF193" s="39"/>
-      <c r="AG193" s="39"/>
-      <c r="AH193" s="39"/>
-      <c r="AI193" s="39"/>
-      <c r="AJ193" s="39"/>
-      <c r="AK193" s="39"/>
-      <c r="AL193" s="39"/>
-      <c r="AM193" s="39"/>
-      <c r="AN193" s="39"/>
-      <c r="AO193" s="39"/>
-      <c r="AP193" s="39"/>
-      <c r="AQ193" s="39"/>
-      <c r="AR193" s="39"/>
-      <c r="AS193" s="39"/>
-      <c r="AT193" s="39"/>
-      <c r="AU193" s="39"/>
-    </row>
-    <row r="194" spans="1:47">
-      <c r="A194" s="39"/>
-      <c r="B194" s="39"/>
-      <c r="C194" s="39"/>
-      <c r="D194" s="39"/>
-      <c r="E194" s="39"/>
-      <c r="F194" s="39"/>
-      <c r="G194" s="39"/>
-      <c r="H194" s="39"/>
-      <c r="I194" s="39"/>
-      <c r="J194" s="39"/>
-      <c r="K194" s="39"/>
-      <c r="L194" s="39"/>
-      <c r="M194" s="39"/>
-      <c r="N194" s="39"/>
-      <c r="O194" s="39"/>
-      <c r="P194" s="39"/>
-      <c r="Q194" s="39"/>
-      <c r="R194" s="39"/>
-      <c r="S194" s="39"/>
-      <c r="T194" s="39"/>
-      <c r="U194" s="39"/>
-      <c r="V194" s="39"/>
-      <c r="W194" s="39"/>
-      <c r="X194" s="39"/>
-      <c r="Y194" s="39"/>
-      <c r="Z194" s="39"/>
-      <c r="AA194" s="39"/>
-      <c r="AB194" s="39"/>
-      <c r="AC194" s="39"/>
-      <c r="AD194" s="39"/>
-      <c r="AE194" s="39"/>
-      <c r="AF194" s="39"/>
-      <c r="AG194" s="39"/>
-      <c r="AH194" s="39"/>
-      <c r="AI194" s="39"/>
-      <c r="AJ194" s="39"/>
-      <c r="AK194" s="39"/>
-      <c r="AL194" s="39"/>
-      <c r="AM194" s="39"/>
-      <c r="AN194" s="39"/>
-      <c r="AO194" s="39"/>
-      <c r="AP194" s="39"/>
-      <c r="AQ194" s="39"/>
-      <c r="AR194" s="39"/>
-      <c r="AS194" s="39"/>
-      <c r="AT194" s="39"/>
-      <c r="AU194" s="39"/>
-    </row>
-    <row r="195" spans="1:47">
-      <c r="A195" s="39"/>
-      <c r="B195" s="39"/>
-      <c r="C195" s="39"/>
-      <c r="D195" s="39"/>
-      <c r="E195" s="39"/>
-      <c r="F195" s="39"/>
-      <c r="G195" s="39"/>
-      <c r="H195" s="39"/>
-      <c r="I195" s="39"/>
-      <c r="J195" s="39"/>
-      <c r="K195" s="39"/>
-      <c r="L195" s="39"/>
-      <c r="M195" s="39"/>
-      <c r="N195" s="39"/>
-      <c r="O195" s="39"/>
-      <c r="P195" s="39"/>
-      <c r="Q195" s="39"/>
-      <c r="R195" s="39"/>
-      <c r="S195" s="39"/>
-      <c r="T195" s="39"/>
-      <c r="U195" s="39"/>
-      <c r="V195" s="39"/>
-      <c r="W195" s="39"/>
-      <c r="X195" s="39"/>
-      <c r="Y195" s="39"/>
-      <c r="Z195" s="39"/>
-      <c r="AA195" s="39"/>
-      <c r="AB195" s="39"/>
-      <c r="AC195" s="39"/>
-      <c r="AD195" s="39"/>
-      <c r="AE195" s="39"/>
-      <c r="AF195" s="39"/>
-      <c r="AG195" s="39"/>
-      <c r="AH195" s="39"/>
-      <c r="AI195" s="39"/>
-      <c r="AJ195" s="39"/>
-      <c r="AK195" s="39"/>
-      <c r="AL195" s="39"/>
-      <c r="AM195" s="39"/>
-      <c r="AN195" s="39"/>
-      <c r="AO195" s="39"/>
-      <c r="AP195" s="39"/>
-      <c r="AQ195" s="39"/>
-      <c r="AR195" s="39"/>
-      <c r="AS195" s="39"/>
-      <c r="AT195" s="39"/>
-      <c r="AU195" s="39"/>
-    </row>
-    <row r="196" spans="1:47">
-      <c r="A196" s="39"/>
-      <c r="B196" s="39"/>
-      <c r="C196" s="39"/>
-      <c r="D196" s="39"/>
-      <c r="E196" s="39"/>
-      <c r="F196" s="39"/>
-      <c r="G196" s="39"/>
-      <c r="H196" s="39"/>
-      <c r="I196" s="39"/>
-      <c r="J196" s="39"/>
-      <c r="K196" s="39"/>
-      <c r="L196" s="39"/>
-      <c r="M196" s="39"/>
-      <c r="N196" s="39"/>
-      <c r="O196" s="39"/>
-      <c r="P196" s="39"/>
-      <c r="Q196" s="39"/>
-      <c r="R196" s="39"/>
-      <c r="S196" s="39"/>
-      <c r="T196" s="39"/>
-      <c r="U196" s="39"/>
-      <c r="V196" s="39"/>
-      <c r="W196" s="39"/>
-      <c r="X196" s="39"/>
-      <c r="Y196" s="39"/>
-      <c r="Z196" s="39"/>
-      <c r="AA196" s="39"/>
-      <c r="AB196" s="39"/>
-      <c r="AC196" s="39"/>
-      <c r="AD196" s="39"/>
-      <c r="AE196" s="39"/>
-      <c r="AF196" s="39"/>
-      <c r="AG196" s="39"/>
-      <c r="AH196" s="39"/>
-      <c r="AI196" s="39"/>
-      <c r="AJ196" s="39"/>
-      <c r="AK196" s="39"/>
-      <c r="AL196" s="39"/>
-      <c r="AM196" s="39"/>
-      <c r="AN196" s="39"/>
-      <c r="AO196" s="39"/>
-      <c r="AP196" s="39"/>
-      <c r="AQ196" s="39"/>
-      <c r="AR196" s="39"/>
-      <c r="AS196" s="39"/>
-      <c r="AT196" s="39"/>
-      <c r="AU196" s="39"/>
-    </row>
-    <row r="197" spans="1:47">
-      <c r="A197" s="39"/>
-      <c r="B197" s="39"/>
-      <c r="C197" s="39"/>
-      <c r="D197" s="39"/>
-      <c r="E197" s="39"/>
-      <c r="F197" s="39"/>
-      <c r="G197" s="39"/>
-      <c r="H197" s="39"/>
-      <c r="I197" s="39"/>
-      <c r="J197" s="39"/>
-      <c r="K197" s="39"/>
-      <c r="L197" s="39"/>
-      <c r="M197" s="39"/>
-      <c r="N197" s="39"/>
-      <c r="O197" s="39"/>
-      <c r="P197" s="39"/>
-      <c r="Q197" s="39"/>
-      <c r="R197" s="39"/>
-      <c r="S197" s="39"/>
-      <c r="T197" s="39"/>
-      <c r="U197" s="39"/>
-      <c r="V197" s="39"/>
-      <c r="W197" s="39"/>
-      <c r="X197" s="39"/>
-      <c r="Y197" s="39"/>
-      <c r="Z197" s="39"/>
-      <c r="AA197" s="39"/>
-      <c r="AB197" s="39"/>
-      <c r="AC197" s="39"/>
-      <c r="AD197" s="39"/>
-      <c r="AE197" s="39"/>
-      <c r="AF197" s="39"/>
-      <c r="AG197" s="39"/>
-      <c r="AH197" s="39"/>
-      <c r="AI197" s="39"/>
-      <c r="AJ197" s="39"/>
-      <c r="AK197" s="39"/>
-      <c r="AL197" s="39"/>
-      <c r="AM197" s="39"/>
-      <c r="AN197" s="39"/>
-      <c r="AO197" s="39"/>
-      <c r="AP197" s="39"/>
-      <c r="AQ197" s="39"/>
-      <c r="AR197" s="39"/>
-      <c r="AS197" s="39"/>
-      <c r="AT197" s="39"/>
-      <c r="AU197" s="39"/>
-    </row>
   </sheetData>
   <autoFilter ref="A22:L22" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
-  <mergeCells count="47">
-    <mergeCell ref="J36:J40"/>
-    <mergeCell ref="K36:K40"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="D36:D40"/>
-    <mergeCell ref="E36:E40"/>
-    <mergeCell ref="F36:F40"/>
-    <mergeCell ref="L36:L40"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="D30:D34"/>
-    <mergeCell ref="E30:E34"/>
-    <mergeCell ref="F30:F34"/>
-    <mergeCell ref="G30:G34"/>
-    <mergeCell ref="H30:H34"/>
-    <mergeCell ref="I30:I34"/>
-    <mergeCell ref="J30:J34"/>
-    <mergeCell ref="K30:K34"/>
-    <mergeCell ref="L30:L34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="G36:G40"/>
-    <mergeCell ref="H36:H40"/>
-    <mergeCell ref="I36:I40"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="D24:D28"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="F24:F28"/>
-    <mergeCell ref="L24:L28"/>
-    <mergeCell ref="B29:D29"/>
+  <mergeCells count="59">
+    <mergeCell ref="J39:J42"/>
+    <mergeCell ref="K39:K42"/>
+    <mergeCell ref="L39:L42"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="L29:L32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="I34:I37"/>
+    <mergeCell ref="J34:J37"/>
+    <mergeCell ref="K34:K37"/>
+    <mergeCell ref="L34:L37"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="G29:G32"/>
+    <mergeCell ref="H29:H32"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="J29:J32"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="L24:L27"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="H21:L21"/>
     <mergeCell ref="B23:D23"/>
-    <mergeCell ref="G24:G28"/>
-    <mergeCell ref="H24:H28"/>
-    <mergeCell ref="I24:I28"/>
-    <mergeCell ref="J24:J28"/>
-    <mergeCell ref="K24:K28"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="K24:K27"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="D39:D42"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="F39:F42"/>
+    <mergeCell ref="G39:G42"/>
+    <mergeCell ref="H39:H42"/>
+    <mergeCell ref="I39:I42"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" sqref="MFX23:MGA40 AMR23:AMU40 SHL23:SHO40 AWN23:AWQ40 MPT23:MPW40 BGJ23:BGM40 VIF23:VII40 BQF23:BQI40 MZP23:MZS40 CAB23:CAE40 SRH23:SRK40 CJX23:CKA40 NJL23:NJO40 CTT23:CTW40 WVP23:WVS40 DDP23:DDS40 NTH23:NTK40 DNL23:DNO40 TBD23:TBG40 DXH23:DXK40 ODD23:ODG40 EHD23:EHG40 VSB23:VSE40 EQZ23:ERC40 OMZ23:ONC40 FAV23:FAY40 TKZ23:TLC40 FKR23:FKU40 OWV23:OWY40 FUN23:FUQ40 JD23:JG40 GEJ23:GEM40 PGR23:PGU40 GOF23:GOI40 TUV23:TUY40 GYB23:GYE40 PQN23:PQQ40 HHX23:HIA40 WBX23:WCA40 HRT23:HRW40 QAJ23:QAM40 IBP23:IBS40 UER23:UEU40 ILL23:ILO40 QKF23:QKI40 IVH23:IVK40 SZ23:TC40 JFD23:JFG40 QUB23:QUE40 JOZ23:JPC40 UON23:UOQ40 JYV23:JYY40 RDX23:REA40 KIR23:KIU40 WLT23:WLW40 KSN23:KSQ40 RNT23:RNW40 LCJ23:LCM40 UYJ23:UYM40 LMF23:LMI40 RXP23:RXS40 LWB23:LWE40 ACV23:ACY40" xr:uid="{56D9884D-EBF1-4FBC-836F-F8753E860E4B}">
-      <formula1>$A$14:$A$19</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H23:L23 H35:L35 H29:L29" xr:uid="{34CAEA61-111B-48A3-802D-71FF1D27517A}">
+    <dataValidation type="list" allowBlank="1" sqref="H23:L23 H28:L28 H33:L33 H38:L38" xr:uid="{34CAEA61-111B-48A3-802D-71FF1D27517A}">
       <formula1>$B$13:$G$13</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{6B022204-3417-4E09-9758-A54C5ECF712A}">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation showDropDown="1" showErrorMessage="1" sqref="JE21:JG22 TA21:TC22 ACW21:ACY22 AMS21:AMU22 AWO21:AWQ22 BGK21:BGM22 BQG21:BQI22 CAC21:CAE22 CJY21:CKA22 CTU21:CTW22 DDQ21:DDS22 DNM21:DNO22 DXI21:DXK22 EHE21:EHG22 ERA21:ERC22 FAW21:FAY22 FKS21:FKU22 FUO21:FUQ22 GEK21:GEM22 GOG21:GOI22 GYC21:GYE22 HHY21:HIA22 HRU21:HRW22 IBQ21:IBS22 ILM21:ILO22 IVI21:IVK22 JFE21:JFG22 JPA21:JPC22 JYW21:JYY22 KIS21:KIU22 KSO21:KSQ22 LCK21:LCM22 LMG21:LMI22 LWC21:LWE22 MFY21:MGA22 MPU21:MPW22 MZQ21:MZS22 NJM21:NJO22 NTI21:NTK22 ODE21:ODG22 ONA21:ONC22 OWW21:OWY22 PGS21:PGU22 PQO21:PQQ22 QAK21:QAM22 QKG21:QKI22 QUC21:QUE22 RDY21:REA22 RNU21:RNW22 RXQ21:RXS22 SHM21:SHO22 SRI21:SRK22 TBE21:TBG22 TLA21:TLC22 TUW21:TUY22 UES21:UEU22 UOO21:UOQ22 UYK21:UYM22 VIG21:VII22 VSC21:VSE22 WBY21:WCA22 WLU21:WLW22 WVQ21:WVS22 H21 H22:L22" xr:uid="{8E845EB7-48A3-46EF-9A04-31CE976BDC12}"/>
+    <dataValidation type="list" allowBlank="1" sqref="ACV23:ACY42 LWB23:LWE42 RXP23:RXS42 LMF23:LMI42 UYJ23:UYM42 LCJ23:LCM42 RNT23:RNW42 KSN23:KSQ42 WLT23:WLW42 KIR23:KIU42 RDX23:REA42 JYV23:JYY42 UON23:UOQ42 JOZ23:JPC42 QUB23:QUE42 JFD23:JFG42 SZ23:TC42 IVH23:IVK42 QKF23:QKI42 ILL23:ILO42 UER23:UEU42 IBP23:IBS42 QAJ23:QAM42 HRT23:HRW42 WBX23:WCA42 HHX23:HIA42 PQN23:PQQ42 GYB23:GYE42 TUV23:TUY42 GOF23:GOI42 PGR23:PGU42 GEJ23:GEM42 JD23:JG42 FUN23:FUQ42 OWV23:OWY42 FKR23:FKU42 TKZ23:TLC42 FAV23:FAY42 OMZ23:ONC42 EQZ23:ERC42 VSB23:VSE42 EHD23:EHG42 ODD23:ODG42 DXH23:DXK42 TBD23:TBG42 DNL23:DNO42 NTH23:NTK42 DDP23:DDS42 WVP23:WVS42 CTT23:CTW42 NJL23:NJO42 CJX23:CKA42 SRH23:SRK42 CAB23:CAE42 MZP23:MZS42 BQF23:BQI42 VIF23:VII42 BGJ23:BGM42 MPT23:MPW42 AWN23:AWQ42 SHL23:SHO42 AMR23:AMU42 MFX23:MGA42" xr:uid="{56D9884D-EBF1-4FBC-836F-F8753E860E4B}">
+      <formula1>$A$14:$A$19</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A23 A29 A35" numberStoredAsText="1"/>
+    <ignoredError sqref="A23 A28 A33" numberStoredAsText="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>

<commit_message>
Update TS for TC001 sort func
</commit_message>
<xml_diff>
--- a/UC02 SortSneakers_BossGiay_TCs.xlsx
+++ b/UC02 SortSneakers_BossGiay_TCs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SENIUM WITH JAVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A794011-771C-425F-8E05-B594D67822EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA428AF4-97C2-4334-8065-272B50182A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{E28AEBC4-528C-4190-9FEA-BFE86C8B68D0}"/>
   </bookViews>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="68">
   <si>
     <t>Environment</t>
   </si>
@@ -465,6 +465,9 @@
       <t xml:space="preserve">
 </t>
     </r>
+  </si>
+  <si>
+    <t>004</t>
   </si>
 </sst>
 </file>
@@ -932,6 +935,15 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="9" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -950,23 +962,8 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -976,6 +973,12 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1674,8 +1677,8 @@
   </sheetPr>
   <dimension ref="A1:AU180"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G93" sqref="G93"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" outlineLevelRow="1"/>
@@ -1703,28 +1706,28 @@
     </row>
     <row r="2" spans="1:13" s="8" customFormat="1" ht="24.6">
       <c r="A2" s="11"/>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
       <c r="H2" s="12"/>
       <c r="M2" s="13"/>
     </row>
     <row r="3" spans="1:13" s="8" customFormat="1" ht="22.8">
       <c r="A3" s="11"/>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="59"/>
+      <c r="C3" s="57"/>
       <c r="D3" s="14"/>
-      <c r="F3" s="60" t="s">
+      <c r="F3" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="60"/>
+      <c r="G3" s="58"/>
       <c r="I3" s="14"/>
       <c r="J3" s="15"/>
       <c r="M3" s="13"/>
@@ -1823,11 +1826,11 @@
       <c r="A10" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="56">
+      <c r="B10" s="59">
         <v>44532</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
@@ -1841,9 +1844,9 @@
       <c r="A11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="56"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
@@ -1885,27 +1888,27 @@
         <v>Build1</v>
       </c>
       <c r="B14" s="25">
-        <f>COUNTIF($L$23:$L$48507,B13)</f>
+        <f t="shared" ref="B14:G14" si="0">COUNTIF($L$23:$L$48507,B13)</f>
         <v>0</v>
       </c>
       <c r="C14" s="25">
-        <f>COUNTIF($L$23:$L$48507,C13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D14" s="25">
-        <f>COUNTIF($L$23:$L$48507,D13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E14" s="25">
-        <f>COUNTIF($L$23:$L$48507,E13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F14" s="25">
-        <f>COUNTIF($L$23:$L$48507,F13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G14" s="25">
-        <f>COUNTIF($L$23:$L$48507,G13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H14" s="26"/>
@@ -1920,27 +1923,27 @@
         <v>Build2</v>
       </c>
       <c r="B15" s="25">
-        <f>COUNTIF($K$23:$K$48507,B13)</f>
+        <f t="shared" ref="B15:G15" si="1">COUNTIF($K$23:$K$48507,B13)</f>
         <v>0</v>
       </c>
       <c r="C15" s="25">
-        <f>COUNTIF($K$23:$K$48507,C13)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D15" s="25">
-        <f>COUNTIF($K$23:$K$48507,D13)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E15" s="25">
-        <f>COUNTIF($K$23:$K$48507,E13)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F15" s="25">
-        <f>COUNTIF($K$23:$K$48507,F13)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G15" s="25">
-        <f>COUNTIF($K$23:$K$48507,G13)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H15" s="26"/>
@@ -2024,27 +2027,27 @@
         <v>Build5</v>
       </c>
       <c r="B18" s="25">
-        <f>COUNTIF($H$23:$H$48507,B13)</f>
+        <f t="shared" ref="B18:G18" si="2">COUNTIF($H$23:$H$48507,B13)</f>
         <v>4</v>
       </c>
       <c r="C18" s="25">
-        <f>COUNTIF($H$23:$H$48507,C13)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D18" s="25">
-        <f>COUNTIF($H$23:$H$48507,D13)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E18" s="25">
-        <f>COUNTIF($H$23:$H$48507,E13)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F18" s="25">
-        <f>COUNTIF($H$23:$H$48507,F13)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G18" s="25">
-        <f>COUNTIF($H$23:$H$48507,G13)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H18" s="26"/>
@@ -2058,27 +2061,27 @@
         <v>24</v>
       </c>
       <c r="B19" s="28">
-        <f t="shared" ref="B19:G19" si="0">SUM(B14:B18)</f>
+        <f t="shared" ref="B19:G19" si="3">SUM(B14:B18)</f>
         <v>4</v>
       </c>
       <c r="C19" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D19" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E19" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F19" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G19" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H19" s="26"/>
@@ -2106,13 +2109,13 @@
       <c r="E21" s="31"/>
       <c r="F21" s="31"/>
       <c r="G21" s="31"/>
-      <c r="H21" s="57" t="s">
+      <c r="H21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="I21" s="57"/>
-      <c r="J21" s="57"/>
-      <c r="K21" s="57"/>
-      <c r="L21" s="57"/>
+      <c r="I21" s="60"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="60"/>
     </row>
     <row r="22" spans="1:12" s="30" customFormat="1" ht="13.2">
       <c r="A22" s="32" t="s">
@@ -2156,11 +2159,11 @@
       <c r="A23" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="53"/>
-      <c r="D23" s="54"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="48"/>
       <c r="E23" s="34"/>
       <c r="F23" s="34"/>
       <c r="G23" s="34"/>
@@ -2173,70 +2176,70 @@
       <c r="L23" s="36"/>
     </row>
     <row r="24" spans="1:12" s="37" customFormat="1" ht="52.2" customHeight="1" outlineLevel="1">
-      <c r="A24" s="46"/>
-      <c r="B24" s="47" t="s">
+      <c r="A24" s="49"/>
+      <c r="B24" s="50" t="s">
         <v>48</v>
       </c>
       <c r="C24" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="48" t="s">
+      <c r="D24" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="49" t="s">
+      <c r="E24" s="52" t="s">
         <v>53</v>
       </c>
       <c r="F24" s="45"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="51"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="54"/>
       <c r="I24" s="45"/>
       <c r="J24" s="45"/>
       <c r="K24" s="45"/>
       <c r="L24" s="45"/>
     </row>
     <row r="25" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A25" s="46"/>
-      <c r="B25" s="47"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="48"/>
-      <c r="E25" s="49"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="52"/>
       <c r="F25" s="45"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="51"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="54"/>
       <c r="I25" s="45"/>
       <c r="J25" s="45"/>
       <c r="K25" s="45"/>
       <c r="L25" s="45"/>
     </row>
     <row r="26" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A26" s="46"/>
-      <c r="B26" s="47"/>
+      <c r="A26" s="49"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="48"/>
-      <c r="E26" s="49"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="52"/>
       <c r="F26" s="45"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="51"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="54"/>
       <c r="I26" s="45"/>
       <c r="J26" s="45"/>
       <c r="K26" s="45"/>
       <c r="L26" s="45"/>
     </row>
     <row r="27" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A27" s="46"/>
-      <c r="B27" s="47"/>
+      <c r="A27" s="49"/>
+      <c r="B27" s="50"/>
       <c r="C27" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="48"/>
-      <c r="E27" s="49"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="52"/>
       <c r="F27" s="45"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="51"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="54"/>
       <c r="I27" s="45"/>
       <c r="J27" s="45"/>
       <c r="K27" s="45"/>
@@ -2246,11 +2249,11 @@
       <c r="A28" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="52" t="s">
+      <c r="B28" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="53"/>
-      <c r="D28" s="54"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="48"/>
       <c r="E28" s="34"/>
       <c r="F28" s="34"/>
       <c r="G28" s="34"/>
@@ -2263,70 +2266,70 @@
       <c r="L28" s="36"/>
     </row>
     <row r="29" spans="1:12" s="37" customFormat="1" ht="52.2" customHeight="1" outlineLevel="1">
-      <c r="A29" s="46"/>
-      <c r="B29" s="47" t="s">
+      <c r="A29" s="49"/>
+      <c r="B29" s="50" t="s">
         <v>48</v>
       </c>
       <c r="C29" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="48" t="s">
+      <c r="D29" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="E29" s="49" t="s">
+      <c r="E29" s="52" t="s">
         <v>53</v>
       </c>
       <c r="F29" s="45"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="51"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="54"/>
       <c r="I29" s="45"/>
       <c r="J29" s="45"/>
       <c r="K29" s="45"/>
       <c r="L29" s="45"/>
     </row>
     <row r="30" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A30" s="46"/>
-      <c r="B30" s="47"/>
+      <c r="A30" s="49"/>
+      <c r="B30" s="50"/>
       <c r="C30" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="48"/>
-      <c r="E30" s="49"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="52"/>
       <c r="F30" s="45"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="51"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="54"/>
       <c r="I30" s="45"/>
       <c r="J30" s="45"/>
       <c r="K30" s="45"/>
       <c r="L30" s="45"/>
     </row>
     <row r="31" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A31" s="46"/>
-      <c r="B31" s="47"/>
+      <c r="A31" s="49"/>
+      <c r="B31" s="50"/>
       <c r="C31" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="48"/>
-      <c r="E31" s="49"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="52"/>
       <c r="F31" s="45"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="51"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="54"/>
       <c r="I31" s="45"/>
       <c r="J31" s="45"/>
       <c r="K31" s="45"/>
       <c r="L31" s="45"/>
     </row>
     <row r="32" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A32" s="46"/>
-      <c r="B32" s="47"/>
+      <c r="A32" s="49"/>
+      <c r="B32" s="50"/>
       <c r="C32" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="48"/>
-      <c r="E32" s="49"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="52"/>
       <c r="F32" s="45"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="51"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="54"/>
       <c r="I32" s="45"/>
       <c r="J32" s="45"/>
       <c r="K32" s="45"/>
@@ -2336,11 +2339,11 @@
       <c r="A33" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="52" t="s">
+      <c r="B33" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="53"/>
-      <c r="D33" s="54"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="48"/>
       <c r="E33" s="34"/>
       <c r="F33" s="34"/>
       <c r="G33" s="34"/>
@@ -2353,70 +2356,70 @@
       <c r="L33" s="36"/>
     </row>
     <row r="34" spans="1:47" s="37" customFormat="1" ht="52.2" customHeight="1" outlineLevel="1">
-      <c r="A34" s="46"/>
-      <c r="B34" s="47" t="s">
+      <c r="A34" s="49"/>
+      <c r="B34" s="50" t="s">
         <v>48</v>
       </c>
       <c r="C34" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="48" t="s">
+      <c r="D34" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="49" t="s">
+      <c r="E34" s="52" t="s">
         <v>53</v>
       </c>
       <c r="F34" s="45"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="51"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="54"/>
       <c r="I34" s="45"/>
       <c r="J34" s="45"/>
       <c r="K34" s="45"/>
       <c r="L34" s="45"/>
     </row>
     <row r="35" spans="1:47" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A35" s="46"/>
-      <c r="B35" s="47"/>
+      <c r="A35" s="49"/>
+      <c r="B35" s="50"/>
       <c r="C35" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="48"/>
-      <c r="E35" s="49"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="52"/>
       <c r="F35" s="45"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="51"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="54"/>
       <c r="I35" s="45"/>
       <c r="J35" s="45"/>
       <c r="K35" s="45"/>
       <c r="L35" s="45"/>
     </row>
     <row r="36" spans="1:47" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A36" s="46"/>
-      <c r="B36" s="47"/>
+      <c r="A36" s="49"/>
+      <c r="B36" s="50"/>
       <c r="C36" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="48"/>
-      <c r="E36" s="49"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="52"/>
       <c r="F36" s="45"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="51"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="54"/>
       <c r="I36" s="45"/>
       <c r="J36" s="45"/>
       <c r="K36" s="45"/>
       <c r="L36" s="45"/>
     </row>
     <row r="37" spans="1:47" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A37" s="46"/>
-      <c r="B37" s="47"/>
+      <c r="A37" s="49"/>
+      <c r="B37" s="50"/>
       <c r="C37" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="48"/>
-      <c r="E37" s="49"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="52"/>
       <c r="F37" s="45"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="51"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="54"/>
       <c r="I37" s="45"/>
       <c r="J37" s="45"/>
       <c r="K37" s="45"/>
@@ -2424,13 +2427,13 @@
     </row>
     <row r="38" spans="1:47" s="18" customFormat="1" ht="13.2">
       <c r="A38" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="53"/>
-      <c r="D38" s="54"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="48"/>
       <c r="E38" s="34"/>
       <c r="F38" s="34"/>
       <c r="G38" s="34"/>
@@ -2443,70 +2446,70 @@
       <c r="L38" s="36"/>
     </row>
     <row r="39" spans="1:47" s="37" customFormat="1" ht="52.2" customHeight="1" outlineLevel="1">
-      <c r="A39" s="46"/>
-      <c r="B39" s="47" t="s">
+      <c r="A39" s="49"/>
+      <c r="B39" s="50" t="s">
         <v>48</v>
       </c>
       <c r="C39" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="48" t="s">
+      <c r="D39" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="E39" s="49" t="s">
+      <c r="E39" s="52" t="s">
         <v>53</v>
       </c>
       <c r="F39" s="45"/>
-      <c r="G39" s="50"/>
-      <c r="H39" s="51"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="54"/>
       <c r="I39" s="45"/>
       <c r="J39" s="45"/>
       <c r="K39" s="45"/>
       <c r="L39" s="45"/>
     </row>
     <row r="40" spans="1:47" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A40" s="46"/>
-      <c r="B40" s="47"/>
+      <c r="A40" s="49"/>
+      <c r="B40" s="50"/>
       <c r="C40" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D40" s="48"/>
-      <c r="E40" s="49"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="52"/>
       <c r="F40" s="45"/>
-      <c r="G40" s="50"/>
-      <c r="H40" s="51"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="54"/>
       <c r="I40" s="45"/>
       <c r="J40" s="45"/>
       <c r="K40" s="45"/>
       <c r="L40" s="45"/>
     </row>
     <row r="41" spans="1:47" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A41" s="46"/>
-      <c r="B41" s="47"/>
+      <c r="A41" s="49"/>
+      <c r="B41" s="50"/>
       <c r="C41" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="D41" s="48"/>
-      <c r="E41" s="49"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="52"/>
       <c r="F41" s="45"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="51"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="54"/>
       <c r="I41" s="45"/>
       <c r="J41" s="45"/>
       <c r="K41" s="45"/>
       <c r="L41" s="45"/>
     </row>
     <row r="42" spans="1:47" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A42" s="46"/>
-      <c r="B42" s="47"/>
+      <c r="A42" s="49"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="D42" s="48"/>
-      <c r="E42" s="49"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="52"/>
       <c r="F42" s="45"/>
-      <c r="G42" s="50"/>
-      <c r="H42" s="51"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="54"/>
       <c r="I42" s="45"/>
       <c r="J42" s="45"/>
       <c r="K42" s="45"/>
@@ -9277,39 +9280,20 @@
   </sheetData>
   <autoFilter ref="A22:L22" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <mergeCells count="59">
-    <mergeCell ref="J39:J42"/>
-    <mergeCell ref="K39:K42"/>
-    <mergeCell ref="L39:L42"/>
-    <mergeCell ref="K29:K32"/>
-    <mergeCell ref="L29:L32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="I34:I37"/>
-    <mergeCell ref="J34:J37"/>
-    <mergeCell ref="K34:K37"/>
-    <mergeCell ref="L34:L37"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="G29:G32"/>
-    <mergeCell ref="H29:H32"/>
-    <mergeCell ref="I29:I32"/>
-    <mergeCell ref="J29:J32"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="F39:F42"/>
+    <mergeCell ref="G39:G42"/>
+    <mergeCell ref="H39:H42"/>
+    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="D39:D42"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="F24:F27"/>
     <mergeCell ref="L24:L27"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
@@ -9322,20 +9306,39 @@
     <mergeCell ref="I24:I27"/>
     <mergeCell ref="J24:J27"/>
     <mergeCell ref="K24:K27"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="D39:D42"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="F39:F42"/>
-    <mergeCell ref="G39:G42"/>
-    <mergeCell ref="H39:H42"/>
-    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="G29:G32"/>
+    <mergeCell ref="H29:H32"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="J29:J32"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="I34:I37"/>
+    <mergeCell ref="J34:J37"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="J39:J42"/>
+    <mergeCell ref="K39:K42"/>
+    <mergeCell ref="L39:L42"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="L29:L32"/>
+    <mergeCell ref="K34:K37"/>
+    <mergeCell ref="L34:L37"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" sqref="H23:L23 H28:L28 H33:L33 H38:L38" xr:uid="{34CAEA61-111B-48A3-802D-71FF1D27517A}">
@@ -9352,7 +9355,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A23 A28 A33" numberStoredAsText="1"/>
+    <ignoredError sqref="A23 A28 A33 A38" numberStoredAsText="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>

<commit_message>
Update TS for TC002 completely
</commit_message>
<xml_diff>
--- a/UC02 SortSneakers_BossGiay_TCs.xlsx
+++ b/UC02 SortSneakers_BossGiay_TCs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SENIUM WITH JAVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA428AF4-97C2-4334-8065-272B50182A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17B131B-BAEA-4498-BAE5-D92847F0E3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{E28AEBC4-528C-4190-9FEA-BFE86C8B68D0}"/>
   </bookViews>
@@ -641,7 +641,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -712,6 +712,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="26"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -810,7 +816,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -935,6 +941,12 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -956,14 +968,14 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -974,11 +986,8 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1677,8 +1686,8 @@
   </sheetPr>
   <dimension ref="A1:AU180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" outlineLevelRow="1"/>
@@ -1706,28 +1715,28 @@
     </row>
     <row r="2" spans="1:13" s="8" customFormat="1" ht="24.6">
       <c r="A2" s="11"/>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
       <c r="H2" s="12"/>
       <c r="M2" s="13"/>
     </row>
     <row r="3" spans="1:13" s="8" customFormat="1" ht="22.8">
       <c r="A3" s="11"/>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="57"/>
+      <c r="C3" s="59"/>
       <c r="D3" s="14"/>
-      <c r="F3" s="58" t="s">
+      <c r="F3" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="58"/>
+      <c r="G3" s="60"/>
       <c r="I3" s="14"/>
       <c r="J3" s="15"/>
       <c r="M3" s="13"/>
@@ -1826,11 +1835,11 @@
       <c r="A10" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="59">
+      <c r="B10" s="56">
         <v>44532</v>
       </c>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
@@ -1844,9 +1853,9 @@
       <c r="A11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
@@ -2028,11 +2037,11 @@
       </c>
       <c r="B18" s="25">
         <f t="shared" ref="B18:G18" si="2">COUNTIF($H$23:$H$48507,B13)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18" s="25">
         <f t="shared" si="2"/>
@@ -2062,11 +2071,11 @@
       </c>
       <c r="B19" s="28">
         <f t="shared" ref="B19:G19" si="3">SUM(B14:B18)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C19" s="28">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D19" s="28">
         <f t="shared" si="3"/>
@@ -2109,13 +2118,13 @@
       <c r="E21" s="31"/>
       <c r="F21" s="31"/>
       <c r="G21" s="31"/>
-      <c r="H21" s="60" t="s">
+      <c r="H21" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="I21" s="60"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="60"/>
-      <c r="L21" s="60"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
     </row>
     <row r="22" spans="1:12" s="30" customFormat="1" ht="13.2">
       <c r="A22" s="32" t="s">
@@ -2159,16 +2168,16 @@
       <c r="A23" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="47"/>
-      <c r="D23" s="48"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="50"/>
       <c r="E23" s="34"/>
       <c r="F23" s="34"/>
       <c r="G23" s="34"/>
-      <c r="H23" s="35" t="s">
-        <v>4</v>
+      <c r="H23" s="61" t="s">
+        <v>5</v>
       </c>
       <c r="I23" s="36"/>
       <c r="J23" s="36"/>
@@ -2176,70 +2185,70 @@
       <c r="L23" s="36"/>
     </row>
     <row r="24" spans="1:12" s="37" customFormat="1" ht="52.2" customHeight="1" outlineLevel="1">
-      <c r="A24" s="49"/>
-      <c r="B24" s="50" t="s">
+      <c r="A24" s="51"/>
+      <c r="B24" s="52" t="s">
         <v>48</v>
       </c>
       <c r="C24" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="51" t="s">
+      <c r="D24" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="52" t="s">
+      <c r="E24" s="54" t="s">
         <v>53</v>
       </c>
       <c r="F24" s="45"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="54"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="47"/>
       <c r="I24" s="45"/>
       <c r="J24" s="45"/>
       <c r="K24" s="45"/>
       <c r="L24" s="45"/>
     </row>
     <row r="25" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A25" s="49"/>
-      <c r="B25" s="50"/>
+      <c r="A25" s="51"/>
+      <c r="B25" s="52"/>
       <c r="C25" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="51"/>
-      <c r="E25" s="52"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="54"/>
       <c r="F25" s="45"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="54"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="47"/>
       <c r="I25" s="45"/>
       <c r="J25" s="45"/>
       <c r="K25" s="45"/>
       <c r="L25" s="45"/>
     </row>
     <row r="26" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A26" s="49"/>
-      <c r="B26" s="50"/>
+      <c r="A26" s="51"/>
+      <c r="B26" s="52"/>
       <c r="C26" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="51"/>
-      <c r="E26" s="52"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="54"/>
       <c r="F26" s="45"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="54"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="47"/>
       <c r="I26" s="45"/>
       <c r="J26" s="45"/>
       <c r="K26" s="45"/>
       <c r="L26" s="45"/>
     </row>
     <row r="27" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A27" s="49"/>
-      <c r="B27" s="50"/>
+      <c r="A27" s="51"/>
+      <c r="B27" s="52"/>
       <c r="C27" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="51"/>
-      <c r="E27" s="52"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="54"/>
       <c r="F27" s="45"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="54"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="47"/>
       <c r="I27" s="45"/>
       <c r="J27" s="45"/>
       <c r="K27" s="45"/>
@@ -2249,16 +2258,16 @@
       <c r="A28" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="46" t="s">
+      <c r="B28" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="47"/>
-      <c r="D28" s="48"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="50"/>
       <c r="E28" s="34"/>
       <c r="F28" s="34"/>
       <c r="G28" s="34"/>
-      <c r="H28" s="35" t="s">
-        <v>4</v>
+      <c r="H28" s="61" t="s">
+        <v>5</v>
       </c>
       <c r="I28" s="36"/>
       <c r="J28" s="36"/>
@@ -2266,70 +2275,70 @@
       <c r="L28" s="36"/>
     </row>
     <row r="29" spans="1:12" s="37" customFormat="1" ht="52.2" customHeight="1" outlineLevel="1">
-      <c r="A29" s="49"/>
-      <c r="B29" s="50" t="s">
+      <c r="A29" s="51"/>
+      <c r="B29" s="52" t="s">
         <v>48</v>
       </c>
       <c r="C29" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="51" t="s">
+      <c r="D29" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="E29" s="52" t="s">
+      <c r="E29" s="54" t="s">
         <v>53</v>
       </c>
       <c r="F29" s="45"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="54"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="47"/>
       <c r="I29" s="45"/>
       <c r="J29" s="45"/>
       <c r="K29" s="45"/>
       <c r="L29" s="45"/>
     </row>
     <row r="30" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A30" s="49"/>
-      <c r="B30" s="50"/>
+      <c r="A30" s="51"/>
+      <c r="B30" s="52"/>
       <c r="C30" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="51"/>
-      <c r="E30" s="52"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="54"/>
       <c r="F30" s="45"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="54"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
       <c r="I30" s="45"/>
       <c r="J30" s="45"/>
       <c r="K30" s="45"/>
       <c r="L30" s="45"/>
     </row>
     <row r="31" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A31" s="49"/>
-      <c r="B31" s="50"/>
+      <c r="A31" s="51"/>
+      <c r="B31" s="52"/>
       <c r="C31" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="51"/>
-      <c r="E31" s="52"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="54"/>
       <c r="F31" s="45"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="54"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="47"/>
       <c r="I31" s="45"/>
       <c r="J31" s="45"/>
       <c r="K31" s="45"/>
       <c r="L31" s="45"/>
     </row>
     <row r="32" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A32" s="49"/>
-      <c r="B32" s="50"/>
+      <c r="A32" s="51"/>
+      <c r="B32" s="52"/>
       <c r="C32" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="51"/>
-      <c r="E32" s="52"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="54"/>
       <c r="F32" s="45"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="54"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="47"/>
       <c r="I32" s="45"/>
       <c r="J32" s="45"/>
       <c r="K32" s="45"/>
@@ -2339,11 +2348,11 @@
       <c r="A33" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="46" t="s">
+      <c r="B33" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="47"/>
-      <c r="D33" s="48"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="50"/>
       <c r="E33" s="34"/>
       <c r="F33" s="34"/>
       <c r="G33" s="34"/>
@@ -2356,70 +2365,70 @@
       <c r="L33" s="36"/>
     </row>
     <row r="34" spans="1:47" s="37" customFormat="1" ht="52.2" customHeight="1" outlineLevel="1">
-      <c r="A34" s="49"/>
-      <c r="B34" s="50" t="s">
+      <c r="A34" s="51"/>
+      <c r="B34" s="52" t="s">
         <v>48</v>
       </c>
       <c r="C34" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="51" t="s">
+      <c r="D34" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="52" t="s">
+      <c r="E34" s="54" t="s">
         <v>53</v>
       </c>
       <c r="F34" s="45"/>
-      <c r="G34" s="53"/>
-      <c r="H34" s="54"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="47"/>
       <c r="I34" s="45"/>
       <c r="J34" s="45"/>
       <c r="K34" s="45"/>
       <c r="L34" s="45"/>
     </row>
     <row r="35" spans="1:47" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A35" s="49"/>
-      <c r="B35" s="50"/>
+      <c r="A35" s="51"/>
+      <c r="B35" s="52"/>
       <c r="C35" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="51"/>
-      <c r="E35" s="52"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="54"/>
       <c r="F35" s="45"/>
-      <c r="G35" s="53"/>
-      <c r="H35" s="54"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="47"/>
       <c r="I35" s="45"/>
       <c r="J35" s="45"/>
       <c r="K35" s="45"/>
       <c r="L35" s="45"/>
     </row>
     <row r="36" spans="1:47" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A36" s="49"/>
-      <c r="B36" s="50"/>
+      <c r="A36" s="51"/>
+      <c r="B36" s="52"/>
       <c r="C36" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="51"/>
-      <c r="E36" s="52"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="54"/>
       <c r="F36" s="45"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="54"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="47"/>
       <c r="I36" s="45"/>
       <c r="J36" s="45"/>
       <c r="K36" s="45"/>
       <c r="L36" s="45"/>
     </row>
     <row r="37" spans="1:47" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A37" s="49"/>
-      <c r="B37" s="50"/>
+      <c r="A37" s="51"/>
+      <c r="B37" s="52"/>
       <c r="C37" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="51"/>
-      <c r="E37" s="52"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="54"/>
       <c r="F37" s="45"/>
-      <c r="G37" s="53"/>
-      <c r="H37" s="54"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="47"/>
       <c r="I37" s="45"/>
       <c r="J37" s="45"/>
       <c r="K37" s="45"/>
@@ -2429,11 +2438,11 @@
       <c r="A38" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="47"/>
-      <c r="D38" s="48"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="50"/>
       <c r="E38" s="34"/>
       <c r="F38" s="34"/>
       <c r="G38" s="34"/>
@@ -2446,70 +2455,70 @@
       <c r="L38" s="36"/>
     </row>
     <row r="39" spans="1:47" s="37" customFormat="1" ht="52.2" customHeight="1" outlineLevel="1">
-      <c r="A39" s="49"/>
-      <c r="B39" s="50" t="s">
+      <c r="A39" s="51"/>
+      <c r="B39" s="52" t="s">
         <v>48</v>
       </c>
       <c r="C39" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="51" t="s">
+      <c r="D39" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="E39" s="52" t="s">
+      <c r="E39" s="54" t="s">
         <v>53</v>
       </c>
       <c r="F39" s="45"/>
-      <c r="G39" s="53"/>
-      <c r="H39" s="54"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="47"/>
       <c r="I39" s="45"/>
       <c r="J39" s="45"/>
       <c r="K39" s="45"/>
       <c r="L39" s="45"/>
     </row>
     <row r="40" spans="1:47" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A40" s="49"/>
-      <c r="B40" s="50"/>
+      <c r="A40" s="51"/>
+      <c r="B40" s="52"/>
       <c r="C40" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D40" s="51"/>
-      <c r="E40" s="52"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="54"/>
       <c r="F40" s="45"/>
-      <c r="G40" s="53"/>
-      <c r="H40" s="54"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="47"/>
       <c r="I40" s="45"/>
       <c r="J40" s="45"/>
       <c r="K40" s="45"/>
       <c r="L40" s="45"/>
     </row>
     <row r="41" spans="1:47" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A41" s="49"/>
-      <c r="B41" s="50"/>
+      <c r="A41" s="51"/>
+      <c r="B41" s="52"/>
       <c r="C41" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="D41" s="51"/>
-      <c r="E41" s="52"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="54"/>
       <c r="F41" s="45"/>
-      <c r="G41" s="53"/>
-      <c r="H41" s="54"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="47"/>
       <c r="I41" s="45"/>
       <c r="J41" s="45"/>
       <c r="K41" s="45"/>
       <c r="L41" s="45"/>
     </row>
     <row r="42" spans="1:47" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A42" s="49"/>
-      <c r="B42" s="50"/>
+      <c r="A42" s="51"/>
+      <c r="B42" s="52"/>
       <c r="C42" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="D42" s="51"/>
-      <c r="E42" s="52"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="54"/>
       <c r="F42" s="45"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="54"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="47"/>
       <c r="I42" s="45"/>
       <c r="J42" s="45"/>
       <c r="K42" s="45"/>
@@ -9280,19 +9289,31 @@
   </sheetData>
   <autoFilter ref="A22:L22" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <mergeCells count="59">
-    <mergeCell ref="F39:F42"/>
-    <mergeCell ref="G39:G42"/>
-    <mergeCell ref="H39:H42"/>
-    <mergeCell ref="I39:I42"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="D39:D42"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="L29:L32"/>
+    <mergeCell ref="K34:K37"/>
+    <mergeCell ref="L34:L37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="J39:J42"/>
+    <mergeCell ref="K39:K42"/>
+    <mergeCell ref="L39:L42"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="I34:I37"/>
+    <mergeCell ref="J34:J37"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="G29:G32"/>
+    <mergeCell ref="H29:H32"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="J29:J32"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
     <mergeCell ref="F24:F27"/>
     <mergeCell ref="L24:L27"/>
     <mergeCell ref="B8:D8"/>
@@ -9306,42 +9327,30 @@
     <mergeCell ref="I24:I27"/>
     <mergeCell ref="J24:J27"/>
     <mergeCell ref="K24:K27"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="D39:D42"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="E24:E27"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="A29:A32"/>
     <mergeCell ref="B29:B32"/>
     <mergeCell ref="D29:D32"/>
     <mergeCell ref="E29:E32"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="G29:G32"/>
-    <mergeCell ref="H29:H32"/>
-    <mergeCell ref="I29:I32"/>
-    <mergeCell ref="J29:J32"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="I34:I37"/>
-    <mergeCell ref="J34:J37"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="A34:A37"/>
     <mergeCell ref="B34:B37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="J39:J42"/>
-    <mergeCell ref="K39:K42"/>
-    <mergeCell ref="L39:L42"/>
-    <mergeCell ref="K29:K32"/>
-    <mergeCell ref="L29:L32"/>
-    <mergeCell ref="K34:K37"/>
-    <mergeCell ref="L34:L37"/>
+    <mergeCell ref="F39:F42"/>
+    <mergeCell ref="G39:G42"/>
+    <mergeCell ref="H39:H42"/>
+    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="B38:D38"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" sqref="H23:L23 H28:L28 H33:L33 H38:L38" xr:uid="{34CAEA61-111B-48A3-802D-71FF1D27517A}">
+    <dataValidation type="list" allowBlank="1" sqref="H23:L23 H38:L38 H33:L33 H28:L28" xr:uid="{34CAEA61-111B-48A3-802D-71FF1D27517A}">
       <formula1>$B$13:$G$13</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{6B022204-3417-4E09-9758-A54C5ECF712A}">

</xml_diff>